<commit_message>
Updating results for bac_test_only
</commit_message>
<xml_diff>
--- a/replication/results/table6_panel2.xlsx
+++ b/replication/results/table6_panel2.xlsx
@@ -43,10 +43,10 @@
     <t>bac_test_primary</t>
   </si>
   <si>
-    <t>(1.12)</t>
-  </si>
-  <si>
-    <t>(0.99)</t>
+    <t>(1.3)</t>
+  </si>
+  <si>
+    <t>(1.05)</t>
   </si>
   <si>
     <t>(0.005)</t>
@@ -55,13 +55,13 @@
     <t>multiple_imputation</t>
   </si>
   <si>
-    <t>(0.49)</t>
-  </si>
-  <si>
-    <t>(0.4)</t>
-  </si>
-  <si>
-    <t>(0.002)</t>
+    <t>(0.62)</t>
+  </si>
+  <si>
+    <t>(0.5)</t>
+  </si>
+  <si>
+    <t>(0.003)</t>
   </si>
 </sst>
 </file>
@@ -452,7 +452,7 @@
         <v>14.25</v>
       </c>
       <c r="C3">
-        <v>15.15</v>
+        <v>15.1</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -474,7 +474,7 @@
         <v>14.66</v>
       </c>
       <c r="C5">
-        <v>14.98</v>
+        <v>15.21</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -496,7 +496,7 @@
         <v>0.081</v>
       </c>
       <c r="C7">
-        <v>0.068</v>
+        <v>0.104</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -518,7 +518,7 @@
         <v>1594</v>
       </c>
       <c r="C9">
-        <v>7200</v>
+        <v>6533</v>
       </c>
     </row>
   </sheetData>

</xml_diff>